<commit_message>
used pandas instead of openpyxl for reading excel
</commit_message>
<xml_diff>
--- a/Data/vanity check.xlsx
+++ b/Data/vanity check.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952D3C42-42F6-4782-9649-DC7821D3BED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="20" r:id="rId1"/>
+    <sheet name="Input_Sheet" sheetId="20" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -22,8 +23,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,13 +61,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -104,7 +113,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -138,6 +147,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -172,9 +182,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -347,139 +358,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>9446664666</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9446644664</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8304040404</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>9400110111</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9496662244</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9400200055</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>9400864321</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9496211555</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9495113111</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9495111311</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9495126345</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9495786942</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>9400311148</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9446224622</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9446424642</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8301010101</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9446545546</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>9495159422</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9495159422</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9400454321</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9495222622</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>9495456345</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9495584955</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8547372717</v>
       </c>

</xml_diff>